<commit_message>
3rd commit by Pradnya
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradnya.Gund\Python\EYDET_Automation Framework\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4A56E0-E89F-49E5-B6C2-49990438670A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C3C33F-1A55-49CB-9968-871A66C37423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="70">
   <si>
     <t>Airline_Prefix</t>
   </si>
@@ -184,27 +184,15 @@
     <t>N</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>NC</t>
   </si>
   <si>
-    <t>CB</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
     <t>AMS</t>
   </si>
   <si>
-    <t>176</t>
-  </si>
-  <si>
-    <t>7800005</t>
-  </si>
-  <si>
     <t>1111111</t>
   </si>
   <si>
@@ -238,37 +226,28 @@
     <t>BLR</t>
   </si>
   <si>
-    <t>2000000000</t>
-  </si>
-  <si>
-    <t>SSE</t>
-  </si>
-  <si>
-    <t>1400054002</t>
-  </si>
-  <si>
     <t>2000000003</t>
   </si>
   <si>
-    <t>2000000002</t>
-  </si>
-  <si>
     <t>2000000001</t>
   </si>
   <si>
-    <t>9702470</t>
-  </si>
-  <si>
-    <t>9702471</t>
-  </si>
-  <si>
-    <t>9702472</t>
-  </si>
-  <si>
-    <t>9702473</t>
-  </si>
-  <si>
-    <t>9702474</t>
+    <t>9702479</t>
+  </si>
+  <si>
+    <t>2121212121</t>
+  </si>
+  <si>
+    <t>9702484</t>
+  </si>
+  <si>
+    <t>9702485</t>
+  </si>
+  <si>
+    <t>9702486</t>
+  </si>
+  <si>
+    <t>9702487</t>
   </si>
 </sst>
 </file>
@@ -315,7 +294,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -338,22 +317,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -376,12 +344,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -664,15 +626,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66EBEF5-6C6F-4C55-8AE2-724E5F4FDCCB}">
-  <dimension ref="A1:AC6"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="2" max="3" width="13.90625" customWidth="1"/>
     <col min="10" max="10" width="14.54296875" customWidth="1"/>
     <col min="26" max="26" width="19.1796875" customWidth="1"/>
     <col min="28" max="28" width="16" customWidth="1"/>
@@ -769,22 +731,22 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>16</v>
@@ -796,25 +758,25 @@
         <v>18</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O2" s="13" t="s">
         <v>42</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="Q2" s="13" t="s">
         <v>25</v>
@@ -830,10 +792,10 @@
         <v>600</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="W2" s="13" t="s">
         <v>15</v>
@@ -851,22 +813,22 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>16</v>
@@ -878,25 +840,25 @@
         <v>18</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O3" s="13" t="s">
         <v>42</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="Q3" s="13" t="s">
         <v>25</v>
@@ -912,10 +874,10 @@
         <v>600</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="W3" s="13" t="s">
         <v>15</v>
@@ -933,22 +895,22 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>16</v>
@@ -960,25 +922,25 @@
         <v>18</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O4" s="13" t="s">
         <v>42</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="Q4" s="13" t="s">
         <v>25</v>
@@ -994,10 +956,10 @@
         <v>600</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="W4" s="13" t="s">
         <v>15</v>
@@ -1015,22 +977,22 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>16</v>
@@ -1042,25 +1004,25 @@
         <v>18</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O5" s="13" t="s">
         <v>42</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="Q5" s="13" t="s">
         <v>25</v>
@@ -1076,10 +1038,10 @@
         <v>600</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="W5" s="13" t="s">
         <v>15</v>
@@ -1094,84 +1056,6 @@
       <c r="AA5" s="13"/>
       <c r="AB5" s="12"/>
       <c r="AC5" s="14"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="O6" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P6" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="R6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="S6" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="T6" s="12">
-        <f t="shared" ref="T6" si="1">R6*S6</f>
-        <v>600</v>
-      </c>
-      <c r="U6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="V6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="W6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="X6" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y6" s="12" t="s">
-        <v>38</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1184,7 +1068,7 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1208,7 +1092,7 @@
         <v>45</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -1238,7 +1122,7 @@
         <v>53</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>15</v>
@@ -1247,7 +1131,7 @@
         <v>46</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1277,7 +1161,7 @@
         <v>53</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>41</v>
@@ -1286,7 +1170,7 @@
         <v>47</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1316,16 +1200,16 @@
         <v>53</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>

</xml_diff>

<commit_message>
4th commit by Pradnya
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradnya.Gund\Python\EYDET_Automation Framework\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C3C33F-1A55-49CB-9968-871A66C37423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76D3D3D-0D15-4E59-A359-C2F992FA2429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -238,16 +238,16 @@
     <t>2121212121</t>
   </si>
   <si>
-    <t>9702484</t>
-  </si>
-  <si>
-    <t>9702485</t>
-  </si>
-  <si>
     <t>9702486</t>
   </si>
   <si>
     <t>9702487</t>
+  </si>
+  <si>
+    <t>9702488</t>
+  </si>
+  <si>
+    <t>9702489</t>
   </si>
 </sst>
 </file>
@@ -629,7 +629,7 @@
   <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
5th commit by Pradnya
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradnya.Gund\Python\EYDET_Automation Framework\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76D3D3D-0D15-4E59-A359-C2F992FA2429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F41B8B5-A89E-4DE0-94F4-B2ED0575542B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add_AWB" sheetId="4" r:id="rId1"/>
     <sheet name="View_AWB" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="62">
   <si>
     <t>Airline_Prefix</t>
   </si>
@@ -79,9 +78,6 @@
     <t>Issue_Date</t>
   </si>
   <si>
-    <t>01/01/2024</t>
-  </si>
-  <si>
     <t>MOP_Freight</t>
   </si>
   <si>
@@ -106,9 +102,6 @@
     <t>Carrier</t>
   </si>
   <si>
-    <t>EY</t>
-  </si>
-  <si>
     <t>Unit_Of_Weight</t>
   </si>
   <si>
@@ -139,18 +132,6 @@
     <t>Flight_Number</t>
   </si>
   <si>
-    <t>0000000019</t>
-  </si>
-  <si>
-    <t>JFK</t>
-  </si>
-  <si>
-    <t>LHR</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
     <t>Chargeable_Weight</t>
   </si>
   <si>
@@ -169,9 +150,6 @@
     <t>K</t>
   </si>
   <si>
-    <t>000</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -193,9 +171,6 @@
     <t>AMS</t>
   </si>
   <si>
-    <t>1111111</t>
-  </si>
-  <si>
     <t>ExportBilling_Status</t>
   </si>
   <si>
@@ -238,16 +213,16 @@
     <t>2121212121</t>
   </si>
   <si>
-    <t>9702486</t>
-  </si>
-  <si>
-    <t>9702487</t>
-  </si>
-  <si>
     <t>9702488</t>
   </si>
   <si>
     <t>9702489</t>
+  </si>
+  <si>
+    <t>9702490</t>
+  </si>
+  <si>
+    <t>9702491</t>
   </si>
 </sst>
 </file>
@@ -628,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66EBEF5-6C6F-4C55-8AE2-724E5F4FDCCB}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -654,46 +629,46 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>7</v>
@@ -708,103 +683,103 @@
         <v>10</v>
       </c>
       <c r="W1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AA1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>63</v>
-      </c>
       <c r="K2" s="13" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="Q2" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="T2" s="12">
         <f>R2*S2</f>
         <v>600</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W2" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X2" s="13" t="s">
         <v>11</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="Z2" s="13"/>
       <c r="AA2" s="13"/>
@@ -813,80 +788,80 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>62</v>
-      </c>
       <c r="K3" s="13" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="L3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="Q3" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R3" s="12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="T3" s="12">
         <f t="shared" ref="T3:T5" si="0">R3*S3</f>
         <v>600</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W3" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X3" s="13" t="s">
         <v>11</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="Z3" s="13"/>
       <c r="AA3" s="13"/>
@@ -895,80 +870,80 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>18</v>
-      </c>
       <c r="J4" s="12" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="L4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="Q4" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R4" s="12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="T4" s="12">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W4" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="Y4" s="12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="Z4" s="13"/>
       <c r="AA4" s="13"/>
@@ -977,80 +952,80 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>61</v>
-      </c>
       <c r="E5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="13" t="s">
+      <c r="H5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="I5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="13" t="s">
-        <v>18</v>
-      </c>
       <c r="J5" s="12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="L5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="Q5" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="T5" s="12">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="W5" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>11</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="Z5" s="13"/>
       <c r="AA5" s="13"/>
@@ -1067,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0530513C-09B3-4079-A60F-7AF0C37ED9C9}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1086,13 +1061,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -1119,19 +1094,19 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1158,19 +1133,19 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1197,19 +1172,19 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1237,468 +1212,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919F5F3A-FF0E-4B2F-ACE0-C9FC0707F845}">
-  <dimension ref="A1:AC5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A2" s="7">
-        <v>607</v>
-      </c>
-      <c r="B2" s="7">
-        <v>2222254</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="7">
-        <v>10</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2" s="4">
-        <f>R2*S2</f>
-        <v>600</v>
-      </c>
-      <c r="U2" s="4">
-        <v>10</v>
-      </c>
-      <c r="V2" s="4">
-        <v>10</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y2" s="4">
-        <v>100</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB2" s="7">
-        <v>1111</v>
-      </c>
-      <c r="AC2" s="9">
-        <v>45292</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A3" s="7">
-        <v>607</v>
-      </c>
-      <c r="B3" s="7">
-        <v>2222255</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="7">
-        <v>10</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="T3" s="4">
-        <f>R3*S3</f>
-        <v>600</v>
-      </c>
-      <c r="U3" s="4">
-        <v>10</v>
-      </c>
-      <c r="V3" s="4">
-        <v>10</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y3" s="4">
-        <v>100</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB3" s="7">
-        <v>1111</v>
-      </c>
-      <c r="AC3" s="9">
-        <v>45292</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A4" s="7">
-        <v>607</v>
-      </c>
-      <c r="B4" s="7">
-        <v>2222256</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="7">
-        <v>10</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="T4" s="4">
-        <f>R4*S4</f>
-        <v>600</v>
-      </c>
-      <c r="U4" s="4">
-        <v>10</v>
-      </c>
-      <c r="V4" s="4">
-        <v>10</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y4" s="4">
-        <v>100</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB4" s="7">
-        <v>1111</v>
-      </c>
-      <c r="AC4" s="9">
-        <v>45292</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A5" s="7">
-        <v>607</v>
-      </c>
-      <c r="B5" s="7">
-        <v>2222257</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="7">
-        <v>10</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="S5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="T5" s="4">
-        <f>R5*S5</f>
-        <v>600</v>
-      </c>
-      <c r="U5" s="4">
-        <v>10</v>
-      </c>
-      <c r="V5" s="4">
-        <v>10</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y5" s="4">
-        <v>100</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB5" s="7">
-        <v>1111</v>
-      </c>
-      <c r="AC5" s="9">
-        <v>45292</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
6th commit by Pradnya
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradnya.Gund\Python\EYDET_Automation Framework\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F41B8B5-A89E-4DE0-94F4-B2ED0575542B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AB804E-5E8F-401C-B11E-5771612FA38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add_AWB" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="58">
   <si>
     <t>Airline_Prefix</t>
   </si>
@@ -168,61 +168,49 @@
     <t>10</t>
   </si>
   <si>
-    <t>AMS</t>
-  </si>
-  <si>
     <t>ExportBilling_Status</t>
   </si>
   <si>
-    <t>057</t>
-  </si>
-  <si>
     <t>01/01/2023</t>
   </si>
   <si>
-    <t>MAA</t>
-  </si>
-  <si>
-    <t>INR</t>
-  </si>
-  <si>
-    <t>AF</t>
-  </si>
-  <si>
     <t>200</t>
   </si>
   <si>
-    <t>HSS</t>
-  </si>
-  <si>
-    <t>DEL</t>
-  </si>
-  <si>
-    <t>BLR</t>
-  </si>
-  <si>
-    <t>2000000003</t>
-  </si>
-  <si>
-    <t>2000000001</t>
-  </si>
-  <si>
     <t>9702479</t>
   </si>
   <si>
     <t>2121212121</t>
   </si>
   <si>
-    <t>9702488</t>
-  </si>
-  <si>
-    <t>9702489</t>
-  </si>
-  <si>
-    <t>9702490</t>
-  </si>
-  <si>
-    <t>9702491</t>
+    <t>9702493</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>5454354543</t>
+  </si>
+  <si>
+    <t>DXB</t>
+  </si>
+  <si>
+    <t>AED</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>EK</t>
+  </si>
+  <si>
+    <t>9702496</t>
+  </si>
+  <si>
+    <t>9702497</t>
+  </si>
+  <si>
+    <t>9702498</t>
   </si>
 </sst>
 </file>
@@ -603,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66EBEF5-6C6F-4C55-8AE2-724E5F4FDCCB}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -706,22 +694,22 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>15</v>
@@ -733,16 +721,16 @@
         <v>17</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>42</v>
@@ -751,7 +739,7 @@
         <v>36</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="Q2" s="13" t="s">
         <v>23</v>
@@ -788,13 +776,13 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>51</v>
@@ -803,7 +791,7 @@
         <v>35</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>15</v>
@@ -815,16 +803,16 @@
         <v>17</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>51</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="N3" s="12" t="s">
         <v>42</v>
@@ -833,7 +821,7 @@
         <v>36</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="Q3" s="13" t="s">
         <v>23</v>
@@ -870,22 +858,22 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>15</v>
@@ -897,16 +885,16 @@
         <v>17</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="N4" s="12" t="s">
         <v>42</v>
@@ -915,7 +903,7 @@
         <v>36</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="Q4" s="13" t="s">
         <v>23</v>
@@ -952,22 +940,22 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>15</v>
@@ -982,13 +970,13 @@
         <v>37</v>
       </c>
       <c r="K5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>43</v>
-      </c>
       <c r="M5" s="13" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="N5" s="12" t="s">
         <v>42</v>
@@ -997,7 +985,7 @@
         <v>36</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="Q5" s="13" t="s">
         <v>23</v>
@@ -1042,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0530513C-09B3-4079-A60F-7AF0C37ED9C9}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1067,7 +1055,7 @@
         <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -1094,10 +1082,10 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>
@@ -1133,10 +1121,10 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>35</v>
@@ -1172,10 +1160,10 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>35</v>

</xml_diff>